<commit_message>
Process new dataset MTLoc Dataset but too large to push
</commit_message>
<xml_diff>
--- a/graph/190611_191009.xlsx
+++ b/graph/190611_191009.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiment\graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F12EEA-66EF-42BF-8648-F7EB62236D97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB2D3B4-529D-4AAF-A5D7-3E479C7D0B9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t>DNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,15 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>K. Long et al.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DANN_CORR
-(proposed)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Time variation 2 with few labeled data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -85,6 +76,33 @@
   </si>
   <si>
     <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Long et al.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HistLoc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加總</t>
+  </si>
+  <si>
+    <t>平均值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>計算加總</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>計數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加總</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -164,48 +182,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:strRef>
-          <c:f>工作表1!$D$5</c:f>
-          <c:strCache>
-            <c:ptCount val="1"/>
-            <c:pt idx="0">
-              <c:v>Time variation 2 with few labeled data</c:v>
-            </c:pt>
-          </c:strCache>
-        </c:strRef>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-TW"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -303,9 +280,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$11,工作表1!$D$13:$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -319,14 +296,7 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DANN_CORR
-(proposed)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>AdapLoc</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>K. Long et al.</c:v>
+                  <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -340,10 +310,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$E$7:$E$11,工作表1!$E$13:$E$14)</c:f>
+              <c:f>(工作表1!$E$7:$E$10,工作表1!$E$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -357,9 +327,6 @@
                   <c:v>1.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -462,9 +429,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$11,工作表1!$D$13:$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -478,14 +445,7 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DANN_CORR
-(proposed)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>AdapLoc</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>K. Long et al.</c:v>
+                  <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -499,10 +459,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$F$7:$F$11,工作表1!$F$13:$F$14)</c:f>
+              <c:f>(工作表1!$F$7:$F$10,工作表1!$F$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>3.24</c:v>
                 </c:pt>
@@ -517,9 +477,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.59</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -572,25 +529,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-084D-4EC3-94AA-99652047AF9F}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -658,9 +596,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$11,工作表1!$D$13:$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -674,14 +612,7 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DANN_CORR
-(proposed)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>AdapLoc</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>K. Long et al.</c:v>
+                  <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -695,17 +626,32 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$G$7:$G$11,工作表1!$G$13:$G$14)</c:f>
+              <c:f>(工作表1!$G$7:$G$10,工作表1!$G$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="6">
-                  <c:v>9.77</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>工作表1!$G$13</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-084D-4EC3-94AA-99652047AF9F}"/>
             </c:ext>
@@ -802,9 +748,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$11,工作表1!$D$13:$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -818,14 +764,7 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DANN_CORR
-(proposed)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>AdapLoc</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>K. Long et al.</c:v>
+                  <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -839,13 +778,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$H$7:$H$11,工作表1!$H$13:$H$14)</c:f>
+              <c:f>(工作表1!$H$7:$H$10,工作表1!$H$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="6">
-                  <c:v>12.51</c:v>
-                </c:pt>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -875,47 +811,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:strRef>
-              <c:f>工作表1!$D$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Models</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="zh-TW"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -964,7 +859,6 @@
         <c:axId val="130701824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="7"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1039,7 +933,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="[=6]&quot;12&quot;;[=5]&quot;10&quot;;0" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1218,7 +1112,6 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1236,48 +1129,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:strRef>
-          <c:f>工作表1!$D$22</c:f>
-          <c:strCache>
-            <c:ptCount val="1"/>
-            <c:pt idx="0">
-              <c:v>Time variation 2 with unlabeled data</c:v>
-            </c:pt>
-          </c:strCache>
-        </c:strRef>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-TW"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1375,9 +1227,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$24:$D$28,工作表1!$D$30:$D$31)</c:f>
+              <c:f>(工作表1!$D$24:$D$27,工作表1!$D$31)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -1391,14 +1243,7 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DANN_CORR
-(proposed)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>AdapLoc</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>K. Long et al.</c:v>
+                  <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1412,10 +1257,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$E$24:$E$28,工作表1!$E$30:$E$31)</c:f>
+              <c:f>(工作表1!$E$24:$E$27,工作表1!$E$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1430,12 +1275,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1537,9 +1376,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$24:$D$28,工作表1!$D$30:$D$31)</c:f>
+              <c:f>(工作表1!$D$24:$D$27,工作表1!$D$31)</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -1553,14 +1392,7 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>DANN_CORR
-(proposed)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>AdapLoc</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>K. Long et al.</c:v>
+                  <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1574,10 +1406,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$F$24:$F$28,工作表1!$F$30:$F$31)</c:f>
+              <c:f>(工作表1!$F$24:$F$27,工作表1!$F$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10.01</c:v>
                 </c:pt>
@@ -1592,12 +1424,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.97</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1629,47 +1455,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:strRef>
-              <c:f>工作表1!$D$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Models</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="zh-TW"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1901,6 +1686,1252 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$R$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Source domain (2019-06-11)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$Q$7:$Q$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HistLoc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$R$7:$R$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0CA3-48D0-B087-A905A622F9B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$S$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Target domain (2019-10-09)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$Q$7:$Q$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HistLoc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$S$7:$S$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0CA3-48D0-B087-A905A622F9B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="480369808"/>
+        <c:axId val="265223216"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$T$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$Q$7:$Q$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HistLoc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$T$7:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="1">
+                  <c:v>9.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0CA3-48D0-B087-A905A622F9B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$U$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$Q$7:$Q$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HistLoc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$U$7:$U$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="1">
+                  <c:v>12.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0CA3-48D0-B087-A905A622F9B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="613924512"/>
+        <c:axId val="251110192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="480369808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="265223216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="265223216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="[=3]&quot;9&quot;;[=4]&quot;12&quot;;0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="480369808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="251110192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="15"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="613924512"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="3"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="613924512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="251110192"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$R$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Source domain (2019-06-11)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$Q$24:$Q$26</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HistLoc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$R$24:$R$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-49A7-4593-B876-8D80F737C51E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$S$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Target domain (2019-10-09)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$Q$24:$Q$26</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HistLoc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$S$24:$S$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-49A7-4593-B876-8D80F737C51E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="779914096"/>
+        <c:axId val="658519952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="779914096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="658519952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="658519952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="779914096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1981,6 +3012,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2485,6 +3596,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2997,10 +5114,10 @@
       <xdr:rowOff>108503</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>474282</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>108053</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>143082</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28178</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3033,10 +5150,10 @@
       <xdr:rowOff>187202</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>496467</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>186752</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>165267</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>106877</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3061,6 +5178,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>392025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="圖表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DF2D334-789D-44EA-8B6E-8848E7ABFEB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>377737</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>105412</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="圖表 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A23EAD74-49C1-4D73-942B-877A12E4F417}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3068,19 +5257,19 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.03678</cdr:x>
-      <cdr:y>0.09006</cdr:y>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.00756</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.06887</cdr:x>
-      <cdr:y>0.1572</cdr:y>
+      <cdr:x>0.07644</cdr:x>
+      <cdr:y>0.09827</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="文字方塊 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F5BA8B-34D9-476C-BFAE-416665534B30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9B43F85-8953-4FDC-9D81-7A4495D0E998}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -3088,22 +5277,19 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="265871" y="322192"/>
-          <a:ext cx="231913" cy="240195"/>
+          <a:off x="0" y="19050"/>
+          <a:ext cx="247650" cy="228600"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:sysClr val="window" lastClr="FFFFFF"/>
-        </a:solidFill>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-TW" sz="1000">
+            <a:rPr lang="en-US" altLang="zh-TW" sz="900">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3111,9 +5297,9 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>14</a:t>
+            <a:t>1</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1000">
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="900">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="65000"/>
@@ -3127,19 +5313,19 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.88244</cdr:x>
-      <cdr:y>0.32969</cdr:y>
+      <cdr:x>0.44685</cdr:x>
+      <cdr:y>0.38365</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.95327</cdr:x>
-      <cdr:y>0.36938</cdr:y>
+      <cdr:x>0.60854</cdr:x>
+      <cdr:y>0.4479</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="6" name="雙波浪 5">
+        <cdr:cNvPr id="3" name="雙波浪 2">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FABB7E5-7376-4044-99B0-ADDC8FAA51E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34099253-DB20-4FFC-8CE8-EC4ADFDFEE2C}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -3147,17 +5333,19 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5718216" y="1186884"/>
-          <a:ext cx="458952" cy="142888"/>
+          <a:off x="1447800" y="966788"/>
+          <a:ext cx="523875" cy="161925"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="doubleWave">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:sysClr val="window" lastClr="FFFFFF"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
         </a:ln>
       </cdr:spPr>
       <cdr:style>
@@ -3451,10 +5639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D5:H31"/>
+  <dimension ref="D5:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3464,29 +5652,47 @@
     <col min="6" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" t="s">
+        <v>11</v>
+      </c>
+      <c r="U6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>0</v>
       </c>
@@ -3496,8 +5702,17 @@
       <c r="F7">
         <v>3.24</v>
       </c>
+      <c r="Q7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1.52</v>
+      </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>2</v>
       </c>
@@ -3507,8 +5722,17 @@
       <c r="F8">
         <v>2.35</v>
       </c>
+      <c r="Q8" t="s">
+        <v>13</v>
+      </c>
+      <c r="T8">
+        <v>9.77</v>
+      </c>
+      <c r="U8">
+        <v>12.51</v>
+      </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>3</v>
       </c>
@@ -3518,8 +5742,17 @@
       <c r="F9">
         <v>2.41</v>
       </c>
+      <c r="Q9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0.59</v>
+      </c>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>4</v>
       </c>
@@ -3530,67 +5763,79 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="11" spans="4:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
-        <v>8</v>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>5</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.59</v>
+        <v>0.73</v>
       </c>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0.73</v>
+        <v>1.52</v>
       </c>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>9.77</v>
+      </c>
+      <c r="H13">
+        <v>12.51</v>
+      </c>
+    </row>
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
         <v>0</v>
       </c>
-      <c r="F13">
-        <v>1.52</v>
+      <c r="F14">
+        <v>0.59</v>
       </c>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14">
-        <v>9.77</v>
-      </c>
-      <c r="H14">
-        <v>12.51</v>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>0</v>
       </c>
@@ -3600,8 +5845,17 @@
       <c r="F24">
         <v>10.01</v>
       </c>
+      <c r="Q24" t="s">
+        <v>6</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>10.97</v>
+      </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>2</v>
       </c>
@@ -3611,8 +5865,23 @@
       <c r="F25">
         <v>21.09</v>
       </c>
+      <c r="Q25" t="s">
+        <v>13</v>
+      </c>
+      <c r="R25">
+        <v>29.2</v>
+      </c>
+      <c r="S25">
+        <v>35.61</v>
+      </c>
+      <c r="T25">
+        <v>29.2</v>
+      </c>
+      <c r="U25">
+        <v>35.61</v>
+      </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>3</v>
       </c>
@@ -3622,8 +5891,17 @@
       <c r="F26">
         <v>13.97</v>
       </c>
+      <c r="Q26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>3.49</v>
+      </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>4</v>
       </c>
@@ -3634,54 +5912,54 @@
         <v>5.73</v>
       </c>
     </row>
-    <row r="28" spans="4:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="s">
-        <v>8</v>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>5</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>3.49</v>
+        <v>4.49</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>4.49</v>
+        <v>10.97</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E30">
+        <v>29.2</v>
+      </c>
+      <c r="F30">
+        <v>35.61</v>
+      </c>
+      <c r="G30">
+        <v>29.2</v>
+      </c>
+      <c r="H30">
+        <v>35.61</v>
+      </c>
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31">
         <v>0</v>
       </c>
-      <c r="F30">
-        <v>10.97</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31">
-        <v>29.2</v>
-      </c>
       <c r="F31">
-        <v>35.61</v>
-      </c>
-      <c r="G31">
-        <v>29.2</v>
-      </c>
-      <c r="H31">
-        <v>35.61</v>
+        <v>3.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(1) Lib Dataset (2) evaluate Mall dataset
</commit_message>
<xml_diff>
--- a/graph/190611_191009.xlsx
+++ b/graph/190611_191009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiment\graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB2D3B4-529D-4AAF-A5D7-3E479C7D0B9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DDB4E5-6943-4F7B-81D5-2D0C53FB0D95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>DNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,25 +84,6 @@
   </si>
   <si>
     <t>HistLoc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>加總</t>
-  </si>
-  <si>
-    <t>平均值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>計算加總</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>計數</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>加總</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -280,9 +261,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$12:$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -296,6 +277,12 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
@@ -310,10 +297,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$E$7:$E$10,工作表1!$E$14)</c:f>
+              <c:f>(工作表1!$E$7:$E$10,工作表1!$E$12:$E$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -327,6 +314,9 @@
                   <c:v>1.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -429,9 +419,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$12:$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -445,6 +435,12 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
@@ -459,10 +455,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$F$7:$F$10,工作表1!$F$14)</c:f>
+              <c:f>(工作表1!$F$7:$F$10,工作表1!$F$12:$F$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3.24</c:v>
                 </c:pt>
@@ -476,6 +472,9 @@
                   <c:v>2.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.59</c:v>
                 </c:pt>
               </c:numCache>
@@ -521,7 +520,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -529,6 +528,25 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-52FE-4384-9AB7-1271E3566AB8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -596,9 +614,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$12:$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -612,6 +630,12 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
@@ -626,32 +650,17 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$G$7:$G$10,工作表1!$G$14)</c:f>
+              <c:f>(工作表1!$G$7:$G$10,工作表1!$G$12:$G$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="5">
+                  <c:v>9.77</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:categoryFilterExceptions>
-                <c15:categoryFilterException>
-                  <c15:sqref>工作表1!$G$13</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c15:spPr>
-                  <c15:invertIfNegative val="0"/>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-              </c15:categoryFilterExceptions>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-084D-4EC3-94AA-99652047AF9F}"/>
             </c:ext>
@@ -748,9 +757,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$14)</c:f>
+              <c:f>(工作表1!$D$7:$D$10,工作表1!$D$12:$D$14)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -764,6 +773,12 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
@@ -778,10 +793,13 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$H$7:$H$10,工作表1!$H$14)</c:f>
+              <c:f>(工作表1!$H$7:$H$10,工作表1!$H$12:$H$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
+                <c:pt idx="5">
+                  <c:v>12.51</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -859,6 +877,7 @@
         <c:axId val="130701824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="7"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -933,7 +952,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="[=5]&quot;10&quot;;[=6]&quot;12&quot;;0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1112,6 +1131,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1227,9 +1247,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$24:$D$27,工作表1!$D$31)</c:f>
+              <c:f>(工作表1!$D$24:$D$27,工作表1!$D$29:$D$31)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -1243,6 +1263,12 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
@@ -1257,10 +1283,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$E$24:$E$27,工作表1!$E$31)</c:f>
+              <c:f>(工作表1!$E$24:$E$27,工作表1!$E$29:$E$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1274,6 +1300,12 @@
                   <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1376,9 +1408,9 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$D$24:$D$27,工作表1!$D$31)</c:f>
+              <c:f>(工作表1!$D$24:$D$27,工作表1!$D$29:$D$31)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>DNN</c:v>
                 </c:pt>
@@ -1392,6 +1424,12 @@
                   <c:v>DANN_1DCAE</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>AdapLoc</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Long et al.</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>HistLoc</c:v>
                 </c:pt>
               </c:strCache>
@@ -1406,10 +1444,10 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(工作表1!$F$24:$F$27,工作表1!$F$31)</c:f>
+              <c:f>(工作表1!$F$24:$F$27,工作表1!$F$29:$F$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>10.01</c:v>
                 </c:pt>
@@ -1423,6 +1461,12 @@
                   <c:v>5.73</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>10.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3.49</c:v>
                 </c:pt>
               </c:numCache>
@@ -2378,6 +2422,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="251110192"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5114,8 +5159,8 @@
       <xdr:rowOff>108503</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>143082</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>3882</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28178</xdr:rowOff>
     </xdr:to>
@@ -5150,8 +5195,8 @@
       <xdr:rowOff>187202</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>165267</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>26067</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>106877</xdr:rowOff>
     </xdr:to>
@@ -5254,6 +5299,132 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04855</cdr:x>
+      <cdr:y>0.01742</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.0997</cdr:x>
+      <cdr:y>0.09679</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="文字方塊 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29A57AD8-0E8B-4605-B2CE-8C5386CF2F9C}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="262143" y="43897"/>
+          <a:ext cx="276225" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="900">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>14</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="900">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.75057</cdr:x>
+      <cdr:y>0.28956</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.82289</cdr:x>
+      <cdr:y>0.34626</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="雙波浪 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED585F13-BD89-4172-871D-552EF56DC90D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4053093" y="729697"/>
+          <a:ext cx="390525" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="doubleWave">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -5641,8 +5812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D5:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z36" sqref="Z36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
After oral and modify content
</commit_message>
<xml_diff>
--- a/graph/190611_191009.xlsx
+++ b/graph/190611_191009.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiment\graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74639CA-8FE6-45BE-83F4-10619C955A80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251FBED2-AD40-4B5C-8D33-BC9508CD3EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,14 +185,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="wdDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="accent1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -519,14 +514,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="wdDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="accent1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -538,14 +528,9 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:pattFill prst="wdDnDiag">
-                <a:fgClr>
-                  <a:schemeClr val="accent1"/>
-                </a:fgClr>
-                <a:bgClr>
-                  <a:schemeClr val="bg1"/>
-                </a:bgClr>
-              </a:pattFill>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -1162,14 +1147,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="wdDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="accent1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -5787,7 +5767,7 @@
   <dimension ref="D5:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
plot CDF of all experiments
</commit_message>
<xml_diff>
--- a/graph/190611_191009.xlsx
+++ b/graph/190611_191009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiment\graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251FBED2-AD40-4B5C-8D33-BC9508CD3EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C1192E-27CA-4EEA-A2DC-EB37F2C2D4CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>DNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +84,10 @@
   </si>
   <si>
     <t>HistLoc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FusionDANN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -275,7 +279,7 @@
                   <c:v>AdapLoc</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Long et al.</c:v>
+                  <c:v>FusionDANN</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>HistLoc</c:v>
@@ -433,7 +437,7 @@
                   <c:v>AdapLoc</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Long et al.</c:v>
+                  <c:v>FusionDANN</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>HistLoc</c:v>
@@ -623,7 +627,7 @@
                   <c:v>AdapLoc</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Long et al.</c:v>
+                  <c:v>FusionDANN</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>HistLoc</c:v>
@@ -766,7 +770,7 @@
                   <c:v>AdapLoc</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Long et al.</c:v>
+                  <c:v>FusionDANN</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>HistLoc</c:v>
@@ -1237,7 +1241,7 @@
                   <c:v>AdapLoc</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Long et al.</c:v>
+                  <c:v>FusionDANN</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>HistLoc</c:v>
@@ -1398,7 +1402,7 @@
                   <c:v>AdapLoc</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Long et al.</c:v>
+                  <c:v>FusionDANN</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>HistLoc</c:v>
@@ -5767,7 +5771,7 @@
   <dimension ref="D5:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5912,7 +5916,7 @@
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G13">
         <v>9.77</v>
@@ -6061,7 +6065,7 @@
     </row>
     <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E30">
         <v>29.2</v>

</xml_diff>